<commit_message>
certain filters added to every execution
</commit_message>
<xml_diff>
--- a/crossout_ledger.xlsx
+++ b/crossout_ledger.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis-\Desktop\crossout_market_old\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis-\Desktop\crossout_market\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521BA548-7072-46FC-AFA7-8357658EB8E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA52F143-3B8B-41A4-A1B8-C276622D5D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2490" windowWidth="21840" windowHeight="13140" xr2:uid="{30DF7398-2C6B-4668-992A-0D887901CC93}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -99,13 +99,40 @@
   </si>
   <si>
     <t>Bigram</t>
+  </si>
+  <si>
+    <t>Cheetah</t>
+  </si>
+  <si>
+    <t>Horizon</t>
+  </si>
+  <si>
+    <t>Leech</t>
+  </si>
+  <si>
+    <t>Dun horse</t>
+  </si>
+  <si>
+    <t>Call of the flame</t>
+  </si>
+  <si>
+    <t>r-2 chill</t>
+  </si>
+  <si>
+    <t>exhaust 2</t>
+  </si>
+  <si>
+    <t>supercharger</t>
+  </si>
+  <si>
+    <t>twin wheel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +144,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -516,15 +549,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF9825-9C19-40B6-BA8A-D5EFB9B74EAE}">
-  <dimension ref="B1:I19"/>
+  <dimension ref="B1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -571,12 +604,12 @@
         <v>0.16482679862961561</v>
       </c>
       <c r="H2" s="6">
-        <f>SUM(E2:E19)</f>
-        <v>212.61500000000012</v>
+        <f>SUM(E2:E31)</f>
+        <v>265.1400000000001</v>
       </c>
       <c r="I2" s="6">
-        <f>AVERAGE(F2:F19)</f>
-        <v>0.11177238729450092</v>
+        <f>AVERAGE(F2:F31)</f>
+        <v>0.12609246591750339</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -799,11 +832,11 @@
         <v>50.98</v>
       </c>
       <c r="E14">
-        <f>(0.9*D14)-C14</f>
+        <f t="shared" ref="E14:E28" si="6">(0.9*D14)-C14</f>
         <v>6.7819999999999965</v>
       </c>
       <c r="F14" s="4">
-        <f>E14/C14</f>
+        <f t="shared" ref="F14:F28" si="7">E14/C14</f>
         <v>0.1734526854219948</v>
       </c>
     </row>
@@ -818,11 +851,11 @@
         <v>298.44</v>
       </c>
       <c r="E15">
-        <f>(0.9*D15)-C15</f>
+        <f t="shared" si="6"/>
         <v>53.436000000000007</v>
       </c>
       <c r="F15" s="4">
-        <f>E15/C15</f>
+        <f t="shared" si="7"/>
         <v>0.24835471277189072</v>
       </c>
     </row>
@@ -837,11 +870,11 @@
         <v>237.87</v>
       </c>
       <c r="E16">
-        <f>(0.9*D16)-C16</f>
+        <f t="shared" si="6"/>
         <v>17.893000000000001</v>
       </c>
       <c r="F16" s="4">
-        <f>E16/C16</f>
+        <f t="shared" si="7"/>
         <v>9.120240583108212E-2</v>
       </c>
     </row>
@@ -856,11 +889,11 @@
         <v>133.93</v>
       </c>
       <c r="E17">
-        <f>(0.9*D17)-C17</f>
+        <f t="shared" si="6"/>
         <v>15.427000000000007</v>
       </c>
       <c r="F17" s="4">
-        <f>E17/C17</f>
+        <f t="shared" si="7"/>
         <v>0.14677005042336605</v>
       </c>
     </row>
@@ -875,11 +908,11 @@
         <v>325</v>
       </c>
       <c r="E18">
-        <f>(0.9*D18)-C18</f>
+        <f t="shared" si="6"/>
         <v>-18.410000000000025</v>
       </c>
       <c r="F18" s="4">
-        <f>E18/C18</f>
+        <f t="shared" si="7"/>
         <v>-5.9213277154160443E-2</v>
       </c>
     </row>
@@ -894,15 +927,244 @@
         <v>399.98</v>
       </c>
       <c r="E19">
-        <f>(0.9*D19)-C19</f>
+        <f t="shared" si="6"/>
         <v>33.862000000000023</v>
       </c>
       <c r="F19" s="4">
-        <f>E19/C19</f>
+        <f t="shared" si="7"/>
         <v>0.10383294492824734</v>
       </c>
     </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>268.56</v>
+      </c>
+      <c r="D20">
+        <v>309.88</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="6"/>
+        <v>10.331999999999994</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="7"/>
+        <v>3.8471849865951716E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="D21">
+        <v>41.39</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="6"/>
+        <v>3.9110000000000014</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="7"/>
+        <v>0.11730653869226158</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>78.61</v>
+      </c>
+      <c r="D22">
+        <v>94.97</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="6"/>
+        <v>6.8629999999999995</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="7"/>
+        <v>8.7304414196667082E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>78.61</v>
+      </c>
+      <c r="D23">
+        <v>94.89</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="6"/>
+        <v>6.7909999999999968</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="7"/>
+        <v>8.6388500190815384E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>101.06</v>
+      </c>
+      <c r="D24">
+        <v>119.98</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="6"/>
+        <v>6.921999999999997</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="7"/>
+        <v>6.8493963981792957E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>3.02</v>
+      </c>
+      <c r="D25">
+        <v>4.99</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="6"/>
+        <v>1.4710000000000005</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="7"/>
+        <v>0.48708609271523196</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>32.03</v>
+      </c>
+      <c r="D26">
+        <v>39.47</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="6"/>
+        <v>3.4930000000000021</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10905401186387767</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>12.71</v>
+      </c>
+      <c r="D27">
+        <v>16.48</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="6"/>
+        <v>2.1219999999999999</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="7"/>
+        <v>0.16695515342250195</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28">
+        <v>12.71</v>
+      </c>
+      <c r="D28">
+        <v>16.48</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="6"/>
+        <v>2.1219999999999999</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="7"/>
+        <v>0.16695515342250195</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>12.71</v>
+      </c>
+      <c r="D29">
+        <v>16.48</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E31" si="8">(0.9*D29)-C29</f>
+        <v>2.1219999999999999</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" ref="F29:F31" si="9">E29/C29</f>
+        <v>0.16695515342250195</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>12.58</v>
+      </c>
+      <c r="D30">
+        <v>16.649999999999999</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="8"/>
+        <v>2.4049999999999994</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" si="9"/>
+        <v>0.19117647058823525</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>46.87</v>
+      </c>
+      <c r="D31">
+        <v>56.49</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="8"/>
+        <v>3.9710000000000036</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="9"/>
+        <v>8.4723703861745339E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>